<commit_message>
Planilha de testes pronta
</commit_message>
<xml_diff>
--- a/documentacao/Tecnologia da Informação/Metodologia Scrum v3.xlsx
+++ b/documentacao/Tecnologia da Informação/Metodologia Scrum v3.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="270">
   <si>
     <t xml:space="preserve">ID </t>
   </si>
@@ -808,9 +808,6 @@
     <t>Conectar a página de Login de usuário com o banco de dados</t>
   </si>
   <si>
-    <t>12h</t>
-  </si>
-  <si>
     <t>Documentação</t>
   </si>
   <si>
@@ -866,6 +863,9 @@
   </si>
   <si>
     <t>Fazer a modelagem Lógica do banco de dados</t>
+  </si>
+  <si>
+    <t>13h</t>
   </si>
 </sst>
 </file>
@@ -1412,6 +1412,15 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="20" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1444,15 +1453,6 @@
     </xf>
     <xf numFmtId="20" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2056,7 +2056,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L219"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+    <sheetView topLeftCell="A26" workbookViewId="0">
       <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
@@ -3919,8 +3919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:AD39"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="M44" sqref="M44"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30:L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5233,8 +5233,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B6:AK49"/>
   <sheetViews>
-    <sheetView topLeftCell="G18" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="T49" sqref="T49"/>
+    <sheetView topLeftCell="B5" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
+      <selection activeCell="T38" sqref="T38:Y38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5361,11 +5361,11 @@
         <v>5</v>
       </c>
       <c r="N8" s="87"/>
-      <c r="O8" s="109" t="s">
+      <c r="O8" s="112" t="s">
         <v>195</v>
       </c>
-      <c r="P8" s="110"/>
-      <c r="Q8" s="108" t="s">
+      <c r="P8" s="113"/>
+      <c r="Q8" s="111" t="s">
         <v>227</v>
       </c>
       <c r="R8" s="84"/>
@@ -5407,9 +5407,9 @@
       <c r="L9" s="107"/>
       <c r="M9" s="87"/>
       <c r="N9" s="87"/>
-      <c r="O9" s="111"/>
-      <c r="P9" s="112"/>
-      <c r="Q9" s="108" t="s">
+      <c r="O9" s="114"/>
+      <c r="P9" s="115"/>
+      <c r="Q9" s="111" t="s">
         <v>227</v>
       </c>
       <c r="R9" s="84"/>
@@ -5451,9 +5451,9 @@
       <c r="L10" s="107"/>
       <c r="M10" s="87"/>
       <c r="N10" s="87"/>
-      <c r="O10" s="111"/>
-      <c r="P10" s="112"/>
-      <c r="Q10" s="108" t="s">
+      <c r="O10" s="114"/>
+      <c r="P10" s="115"/>
+      <c r="Q10" s="111" t="s">
         <v>227</v>
       </c>
       <c r="R10" s="84"/>
@@ -5495,9 +5495,9 @@
       <c r="L11" s="107"/>
       <c r="M11" s="87"/>
       <c r="N11" s="87"/>
-      <c r="O11" s="111"/>
-      <c r="P11" s="112"/>
-      <c r="Q11" s="108" t="s">
+      <c r="O11" s="114"/>
+      <c r="P11" s="115"/>
+      <c r="Q11" s="111" t="s">
         <v>227</v>
       </c>
       <c r="R11" s="84"/>
@@ -5539,9 +5539,9 @@
       <c r="L12" s="107"/>
       <c r="M12" s="87"/>
       <c r="N12" s="87"/>
-      <c r="O12" s="111"/>
-      <c r="P12" s="112"/>
-      <c r="Q12" s="108" t="s">
+      <c r="O12" s="114"/>
+      <c r="P12" s="115"/>
+      <c r="Q12" s="111" t="s">
         <v>227</v>
       </c>
       <c r="R12" s="84"/>
@@ -5583,9 +5583,9 @@
       <c r="L13" s="107"/>
       <c r="M13" s="87"/>
       <c r="N13" s="87"/>
-      <c r="O13" s="111"/>
-      <c r="P13" s="112"/>
-      <c r="Q13" s="108" t="s">
+      <c r="O13" s="114"/>
+      <c r="P13" s="115"/>
+      <c r="Q13" s="111" t="s">
         <v>227</v>
       </c>
       <c r="R13" s="84"/>
@@ -5627,9 +5627,9 @@
       <c r="L14" s="107"/>
       <c r="M14" s="87"/>
       <c r="N14" s="87"/>
-      <c r="O14" s="111"/>
-      <c r="P14" s="112"/>
-      <c r="Q14" s="108" t="s">
+      <c r="O14" s="114"/>
+      <c r="P14" s="115"/>
+      <c r="Q14" s="111" t="s">
         <v>227</v>
       </c>
       <c r="R14" s="84"/>
@@ -5671,9 +5671,9 @@
       <c r="L15" s="107"/>
       <c r="M15" s="87"/>
       <c r="N15" s="87"/>
-      <c r="O15" s="111"/>
-      <c r="P15" s="112"/>
-      <c r="Q15" s="108" t="s">
+      <c r="O15" s="114"/>
+      <c r="P15" s="115"/>
+      <c r="Q15" s="111" t="s">
         <v>227</v>
       </c>
       <c r="R15" s="84"/>
@@ -5715,9 +5715,9 @@
       <c r="L16" s="107"/>
       <c r="M16" s="87"/>
       <c r="N16" s="87"/>
-      <c r="O16" s="111"/>
-      <c r="P16" s="112"/>
-      <c r="Q16" s="108" t="s">
+      <c r="O16" s="114"/>
+      <c r="P16" s="115"/>
+      <c r="Q16" s="111" t="s">
         <v>227</v>
       </c>
       <c r="R16" s="84"/>
@@ -5759,9 +5759,9 @@
       <c r="L17" s="107"/>
       <c r="M17" s="87"/>
       <c r="N17" s="87"/>
-      <c r="O17" s="111"/>
-      <c r="P17" s="112"/>
-      <c r="Q17" s="108" t="s">
+      <c r="O17" s="114"/>
+      <c r="P17" s="115"/>
+      <c r="Q17" s="111" t="s">
         <v>227</v>
       </c>
       <c r="R17" s="84"/>
@@ -5807,9 +5807,9 @@
         <v>5</v>
       </c>
       <c r="N18" s="87"/>
-      <c r="O18" s="111"/>
-      <c r="P18" s="112"/>
-      <c r="Q18" s="108" t="s">
+      <c r="O18" s="114"/>
+      <c r="P18" s="115"/>
+      <c r="Q18" s="111" t="s">
         <v>226</v>
       </c>
       <c r="R18" s="84"/>
@@ -5824,9 +5824,8 @@
       <c r="Y18" s="84"/>
       <c r="Z18" s="1"/>
       <c r="AA18" s="1"/>
-      <c r="AB18" s="22"/>
       <c r="AC18" s="1"/>
-      <c r="AD18" s="1"/>
+      <c r="AD18" s="22"/>
       <c r="AE18" s="60"/>
       <c r="AF18" s="60"/>
       <c r="AG18" s="59"/>
@@ -5851,9 +5850,9 @@
       <c r="L19" s="107"/>
       <c r="M19" s="87"/>
       <c r="N19" s="87"/>
-      <c r="O19" s="111"/>
-      <c r="P19" s="112"/>
-      <c r="Q19" s="108" t="s">
+      <c r="O19" s="114"/>
+      <c r="P19" s="115"/>
+      <c r="Q19" s="111" t="s">
         <v>226</v>
       </c>
       <c r="R19" s="84"/>
@@ -5868,9 +5867,8 @@
       <c r="Y19" s="84"/>
       <c r="Z19" s="1"/>
       <c r="AA19" s="1"/>
-      <c r="AB19" s="22"/>
       <c r="AC19" s="1"/>
-      <c r="AD19" s="1"/>
+      <c r="AD19" s="22"/>
       <c r="AE19" s="60"/>
       <c r="AF19" s="60"/>
       <c r="AG19" s="59"/>
@@ -5899,8 +5897,8 @@
         <v>4</v>
       </c>
       <c r="N20" s="87"/>
-      <c r="O20" s="111"/>
-      <c r="P20" s="112"/>
+      <c r="O20" s="114"/>
+      <c r="P20" s="115"/>
       <c r="Q20" s="87" t="s">
         <v>179</v>
       </c>
@@ -5914,11 +5912,11 @@
       <c r="W20" s="103"/>
       <c r="X20" s="103"/>
       <c r="Y20" s="103"/>
-      <c r="Z20" s="115"/>
+      <c r="Z20" s="118"/>
       <c r="AA20" s="69"/>
       <c r="AB20" s="69"/>
       <c r="AC20" s="69"/>
-      <c r="AD20" s="116"/>
+      <c r="AD20" s="119"/>
       <c r="AE20" s="60"/>
       <c r="AF20" s="60"/>
       <c r="AG20" s="59"/>
@@ -5943,8 +5941,8 @@
       <c r="L21" s="107"/>
       <c r="M21" s="87"/>
       <c r="N21" s="87"/>
-      <c r="O21" s="111"/>
-      <c r="P21" s="112"/>
+      <c r="O21" s="114"/>
+      <c r="P21" s="115"/>
       <c r="Q21" s="87"/>
       <c r="R21" s="87"/>
       <c r="S21" s="87"/>
@@ -5954,11 +5952,11 @@
       <c r="W21" s="103"/>
       <c r="X21" s="103"/>
       <c r="Y21" s="103"/>
-      <c r="Z21" s="115"/>
+      <c r="Z21" s="118"/>
       <c r="AA21" s="69"/>
       <c r="AB21" s="69"/>
       <c r="AC21" s="69"/>
-      <c r="AD21" s="116"/>
+      <c r="AD21" s="119"/>
       <c r="AE21" s="60"/>
       <c r="AF21" s="60"/>
       <c r="AG21" s="59"/>
@@ -5987,8 +5985,8 @@
         <v>4</v>
       </c>
       <c r="N22" s="87"/>
-      <c r="O22" s="111"/>
-      <c r="P22" s="112"/>
+      <c r="O22" s="114"/>
+      <c r="P22" s="115"/>
       <c r="Q22" s="87" t="s">
         <v>179</v>
       </c>
@@ -6004,7 +6002,7 @@
       <c r="Y22" s="103"/>
       <c r="Z22" s="69"/>
       <c r="AA22" s="69"/>
-      <c r="AB22" s="115"/>
+      <c r="AB22" s="118"/>
       <c r="AC22" s="69"/>
       <c r="AD22" s="69"/>
       <c r="AE22" s="60"/>
@@ -6031,8 +6029,8 @@
       <c r="L23" s="107"/>
       <c r="M23" s="87"/>
       <c r="N23" s="87"/>
-      <c r="O23" s="111"/>
-      <c r="P23" s="112"/>
+      <c r="O23" s="114"/>
+      <c r="P23" s="115"/>
       <c r="Q23" s="87"/>
       <c r="R23" s="87"/>
       <c r="S23" s="87"/>
@@ -6044,7 +6042,7 @@
       <c r="Y23" s="103"/>
       <c r="Z23" s="69"/>
       <c r="AA23" s="69"/>
-      <c r="AB23" s="115"/>
+      <c r="AB23" s="118"/>
       <c r="AC23" s="69"/>
       <c r="AD23" s="69"/>
       <c r="AE23" s="60"/>
@@ -6071,8 +6069,8 @@
       <c r="L24" s="107"/>
       <c r="M24" s="87"/>
       <c r="N24" s="87"/>
-      <c r="O24" s="111"/>
-      <c r="P24" s="112"/>
+      <c r="O24" s="114"/>
+      <c r="P24" s="115"/>
       <c r="Q24" s="84" t="s">
         <v>180</v>
       </c>
@@ -6119,8 +6117,8 @@
         <v>5</v>
       </c>
       <c r="N25" s="87"/>
-      <c r="O25" s="111"/>
-      <c r="P25" s="112"/>
+      <c r="O25" s="114"/>
+      <c r="P25" s="115"/>
       <c r="Q25" s="87" t="s">
         <v>181</v>
       </c>
@@ -6138,7 +6136,7 @@
       <c r="AA25" s="69"/>
       <c r="AB25" s="69"/>
       <c r="AC25" s="69"/>
-      <c r="AD25" s="115"/>
+      <c r="AD25" s="118"/>
       <c r="AE25" s="60"/>
       <c r="AF25" s="60"/>
       <c r="AG25" s="59"/>
@@ -6163,8 +6161,8 @@
       <c r="L26" s="107"/>
       <c r="M26" s="87"/>
       <c r="N26" s="87"/>
-      <c r="O26" s="111"/>
-      <c r="P26" s="112"/>
+      <c r="O26" s="114"/>
+      <c r="P26" s="115"/>
       <c r="Q26" s="87"/>
       <c r="R26" s="87"/>
       <c r="S26" s="87"/>
@@ -6178,7 +6176,7 @@
       <c r="AA26" s="69"/>
       <c r="AB26" s="69"/>
       <c r="AC26" s="69"/>
-      <c r="AD26" s="115"/>
+      <c r="AD26" s="118"/>
       <c r="AE26" s="60"/>
       <c r="AF26" s="60"/>
       <c r="AG26" s="59"/>
@@ -6203,8 +6201,8 @@
       <c r="L27" s="107"/>
       <c r="M27" s="87"/>
       <c r="N27" s="87"/>
-      <c r="O27" s="111"/>
-      <c r="P27" s="112"/>
+      <c r="O27" s="114"/>
+      <c r="P27" s="115"/>
       <c r="Q27" s="87" t="s">
         <v>181</v>
       </c>
@@ -6222,7 +6220,7 @@
       <c r="AA27" s="69"/>
       <c r="AB27" s="69"/>
       <c r="AC27" s="69"/>
-      <c r="AD27" s="115"/>
+      <c r="AD27" s="118"/>
       <c r="AE27" s="60"/>
       <c r="AF27" s="60"/>
       <c r="AG27" s="59"/>
@@ -6247,8 +6245,8 @@
       <c r="L28" s="107"/>
       <c r="M28" s="87"/>
       <c r="N28" s="87"/>
-      <c r="O28" s="111"/>
-      <c r="P28" s="112"/>
+      <c r="O28" s="114"/>
+      <c r="P28" s="115"/>
       <c r="Q28" s="87"/>
       <c r="R28" s="87"/>
       <c r="S28" s="87"/>
@@ -6262,7 +6260,7 @@
       <c r="AA28" s="69"/>
       <c r="AB28" s="69"/>
       <c r="AC28" s="69"/>
-      <c r="AD28" s="115"/>
+      <c r="AD28" s="118"/>
       <c r="AE28" s="60"/>
       <c r="AF28" s="60"/>
       <c r="AG28" s="59"/>
@@ -6287,8 +6285,8 @@
       <c r="L29" s="107"/>
       <c r="M29" s="87"/>
       <c r="N29" s="87"/>
-      <c r="O29" s="111"/>
-      <c r="P29" s="112"/>
+      <c r="O29" s="114"/>
+      <c r="P29" s="115"/>
       <c r="Q29" s="84" t="s">
         <v>180</v>
       </c>
@@ -6335,8 +6333,8 @@
         <v>4</v>
       </c>
       <c r="N30" s="87"/>
-      <c r="O30" s="111"/>
-      <c r="P30" s="112"/>
+      <c r="O30" s="114"/>
+      <c r="P30" s="115"/>
       <c r="Q30" s="84" t="s">
         <v>183</v>
       </c>
@@ -6379,8 +6377,8 @@
       <c r="L31" s="107"/>
       <c r="M31" s="87"/>
       <c r="N31" s="87"/>
-      <c r="O31" s="111"/>
-      <c r="P31" s="112"/>
+      <c r="O31" s="114"/>
+      <c r="P31" s="115"/>
       <c r="Q31" s="84" t="s">
         <v>182</v>
       </c>
@@ -6423,8 +6421,8 @@
       <c r="L32" s="107"/>
       <c r="M32" s="87"/>
       <c r="N32" s="87"/>
-      <c r="O32" s="113"/>
-      <c r="P32" s="114"/>
+      <c r="O32" s="116"/>
+      <c r="P32" s="117"/>
       <c r="Q32" s="84" t="s">
         <v>182</v>
       </c>
@@ -6500,12 +6498,12 @@
       <c r="F34" s="87"/>
       <c r="G34" s="87"/>
       <c r="H34" s="87"/>
-      <c r="I34" s="119" t="s">
+      <c r="I34" s="108" t="s">
         <v>230</v>
       </c>
-      <c r="J34" s="120"/>
-      <c r="K34" s="120"/>
-      <c r="L34" s="121"/>
+      <c r="J34" s="109"/>
+      <c r="K34" s="109"/>
+      <c r="L34" s="110"/>
       <c r="M34" s="87">
         <v>5</v>
       </c>
@@ -6549,12 +6547,12 @@
       <c r="F35" s="87"/>
       <c r="G35" s="87"/>
       <c r="H35" s="87"/>
-      <c r="I35" s="119" t="s">
+      <c r="I35" s="108" t="s">
         <v>231</v>
       </c>
-      <c r="J35" s="120"/>
-      <c r="K35" s="120"/>
-      <c r="L35" s="121"/>
+      <c r="J35" s="109"/>
+      <c r="K35" s="109"/>
+      <c r="L35" s="110"/>
       <c r="M35" s="87"/>
       <c r="N35" s="87"/>
       <c r="O35" s="87"/>
@@ -6594,12 +6592,12 @@
       <c r="F36" s="87"/>
       <c r="G36" s="87"/>
       <c r="H36" s="87"/>
-      <c r="I36" s="119" t="s">
+      <c r="I36" s="108" t="s">
         <v>232</v>
       </c>
-      <c r="J36" s="120"/>
-      <c r="K36" s="120"/>
-      <c r="L36" s="121"/>
+      <c r="J36" s="109"/>
+      <c r="K36" s="109"/>
+      <c r="L36" s="110"/>
       <c r="M36" s="87"/>
       <c r="N36" s="87"/>
       <c r="O36" s="87"/>
@@ -6639,12 +6637,12 @@
       <c r="F37" s="87"/>
       <c r="G37" s="87"/>
       <c r="H37" s="87"/>
-      <c r="I37" s="119" t="s">
+      <c r="I37" s="108" t="s">
         <v>233</v>
       </c>
-      <c r="J37" s="120"/>
-      <c r="K37" s="120"/>
-      <c r="L37" s="121"/>
+      <c r="J37" s="109"/>
+      <c r="K37" s="109"/>
+      <c r="L37" s="110"/>
       <c r="M37" s="87"/>
       <c r="N37" s="87"/>
       <c r="O37" s="87"/>
@@ -6723,12 +6721,12 @@
       <c r="F39" s="87"/>
       <c r="G39" s="87"/>
       <c r="H39" s="87"/>
-      <c r="I39" s="119" t="s">
+      <c r="I39" s="108" t="s">
         <v>234</v>
       </c>
-      <c r="J39" s="120"/>
-      <c r="K39" s="120"/>
-      <c r="L39" s="121"/>
+      <c r="J39" s="109"/>
+      <c r="K39" s="109"/>
+      <c r="L39" s="110"/>
       <c r="M39" s="87">
         <v>5</v>
       </c>
@@ -6772,12 +6770,12 @@
       <c r="F40" s="87"/>
       <c r="G40" s="87"/>
       <c r="H40" s="87"/>
-      <c r="I40" s="119" t="s">
+      <c r="I40" s="108" t="s">
         <v>236</v>
       </c>
-      <c r="J40" s="120"/>
-      <c r="K40" s="120"/>
-      <c r="L40" s="121"/>
+      <c r="J40" s="109"/>
+      <c r="K40" s="109"/>
+      <c r="L40" s="110"/>
       <c r="M40" s="87"/>
       <c r="N40" s="87"/>
       <c r="O40" s="87"/>
@@ -6860,7 +6858,7 @@
         <v>3</v>
       </c>
       <c r="N42" s="87"/>
-      <c r="O42" s="118" t="s">
+      <c r="O42" s="121" t="s">
         <v>199</v>
       </c>
       <c r="P42" s="87"/>
@@ -6916,8 +6914,8 @@
       <c r="Y43" s="103"/>
       <c r="Z43" s="69"/>
       <c r="AA43" s="69"/>
-      <c r="AB43" s="115"/>
-      <c r="AC43" s="115"/>
+      <c r="AB43" s="118"/>
+      <c r="AC43" s="118"/>
       <c r="AD43" s="69"/>
     </row>
     <row r="44" spans="2:37" x14ac:dyDescent="0.25">
@@ -6949,8 +6947,8 @@
       <c r="Y44" s="103"/>
       <c r="Z44" s="69"/>
       <c r="AA44" s="69"/>
-      <c r="AB44" s="115"/>
-      <c r="AC44" s="115"/>
+      <c r="AB44" s="118"/>
+      <c r="AC44" s="118"/>
       <c r="AD44" s="69"/>
     </row>
     <row r="45" spans="2:37" x14ac:dyDescent="0.25">
@@ -7008,11 +7006,11 @@
       <c r="N46" s="87"/>
       <c r="O46" s="87"/>
       <c r="P46" s="87"/>
-      <c r="Q46" s="117" t="s">
+      <c r="Q46" s="120" t="s">
         <v>196</v>
       </c>
-      <c r="R46" s="117"/>
-      <c r="S46" s="117"/>
+      <c r="R46" s="120"/>
+      <c r="S46" s="120"/>
       <c r="T46" s="84" t="s">
         <v>192</v>
       </c>
@@ -7076,15 +7074,6 @@
     <mergeCell ref="AC27:AC28"/>
     <mergeCell ref="AD27:AD28"/>
     <mergeCell ref="Z25:Z26"/>
-    <mergeCell ref="AA25:AA26"/>
-    <mergeCell ref="AB25:AB26"/>
-    <mergeCell ref="AC25:AC26"/>
-    <mergeCell ref="AD25:AD26"/>
-    <mergeCell ref="Z22:Z23"/>
-    <mergeCell ref="AA22:AA23"/>
-    <mergeCell ref="AB22:AB23"/>
-    <mergeCell ref="AC22:AC23"/>
-    <mergeCell ref="AD22:AD23"/>
     <mergeCell ref="Z20:Z21"/>
     <mergeCell ref="AA20:AA21"/>
     <mergeCell ref="AB20:AB21"/>
@@ -7098,6 +7087,15 @@
     <mergeCell ref="Q24:S24"/>
     <mergeCell ref="Q22:S23"/>
     <mergeCell ref="Q25:S26"/>
+    <mergeCell ref="AA25:AA26"/>
+    <mergeCell ref="AB25:AB26"/>
+    <mergeCell ref="AC25:AC26"/>
+    <mergeCell ref="AD25:AD26"/>
+    <mergeCell ref="Z22:Z23"/>
+    <mergeCell ref="AA22:AA23"/>
+    <mergeCell ref="AB22:AB23"/>
+    <mergeCell ref="AC22:AC23"/>
+    <mergeCell ref="AD22:AD23"/>
     <mergeCell ref="T37:Y37"/>
     <mergeCell ref="T29:Y29"/>
     <mergeCell ref="T30:Y30"/>
@@ -7198,8 +7196,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:AF45"/>
   <sheetViews>
-    <sheetView topLeftCell="D2" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
-      <selection activeCell="P28" sqref="P28"/>
+    <sheetView topLeftCell="C3" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+      <selection activeCell="O36" sqref="O36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7313,22 +7311,22 @@
       </c>
       <c r="O6" s="73"/>
       <c r="P6" s="123" t="s">
-        <v>250</v>
+        <v>269</v>
       </c>
       <c r="Q6" s="123"/>
       <c r="R6" s="122" t="s">
         <v>228</v>
       </c>
-      <c r="S6" s="116"/>
-      <c r="T6" s="116"/>
-      <c r="U6" s="116" t="s">
+      <c r="S6" s="119"/>
+      <c r="T6" s="119"/>
+      <c r="U6" s="119" t="s">
         <v>247</v>
       </c>
-      <c r="V6" s="116"/>
-      <c r="W6" s="116"/>
-      <c r="X6" s="116"/>
-      <c r="Y6" s="116"/>
-      <c r="Z6" s="116"/>
+      <c r="V6" s="119"/>
+      <c r="W6" s="119"/>
+      <c r="X6" s="119"/>
+      <c r="Y6" s="119"/>
+      <c r="Z6" s="119"/>
       <c r="AA6" s="5"/>
       <c r="AB6" s="1"/>
       <c r="AC6" s="22"/>
@@ -7360,16 +7358,16 @@
       <c r="R7" s="122" t="s">
         <v>228</v>
       </c>
-      <c r="S7" s="116"/>
-      <c r="T7" s="116"/>
-      <c r="U7" s="116" t="s">
+      <c r="S7" s="119"/>
+      <c r="T7" s="119"/>
+      <c r="U7" s="119" t="s">
         <v>248</v>
       </c>
-      <c r="V7" s="116"/>
-      <c r="W7" s="116"/>
-      <c r="X7" s="116"/>
-      <c r="Y7" s="116"/>
-      <c r="Z7" s="116"/>
+      <c r="V7" s="119"/>
+      <c r="W7" s="119"/>
+      <c r="X7" s="119"/>
+      <c r="Y7" s="119"/>
+      <c r="Z7" s="119"/>
       <c r="AA7" s="1"/>
       <c r="AB7" s="1"/>
       <c r="AC7" s="22"/>
@@ -7398,7 +7396,9 @@
       <c r="O8" s="73"/>
       <c r="P8" s="123"/>
       <c r="Q8" s="123"/>
-      <c r="R8" s="122"/>
+      <c r="R8" s="122" t="s">
+        <v>184</v>
+      </c>
       <c r="S8" s="122"/>
       <c r="T8" s="122"/>
       <c r="U8" s="125" t="s">
@@ -7558,7 +7558,7 @@
         <v>8</v>
       </c>
       <c r="D13" s="87" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E13" s="87"/>
       <c r="F13" s="87"/>
@@ -7566,7 +7566,7 @@
       <c r="H13" s="87"/>
       <c r="I13" s="87"/>
       <c r="J13" s="124" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="K13" s="124"/>
       <c r="L13" s="124"/>
@@ -7576,27 +7576,26 @@
       </c>
       <c r="O13" s="73"/>
       <c r="P13" s="123" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="Q13" s="123"/>
       <c r="R13" s="122" t="s">
         <v>184</v>
       </c>
-      <c r="S13" s="116"/>
-      <c r="T13" s="116"/>
-      <c r="U13" s="116" t="s">
-        <v>253</v>
-      </c>
-      <c r="V13" s="116"/>
-      <c r="W13" s="116"/>
-      <c r="X13" s="116"/>
-      <c r="Y13" s="116"/>
-      <c r="Z13" s="116"/>
+      <c r="S13" s="119"/>
+      <c r="T13" s="119"/>
+      <c r="U13" s="119" t="s">
+        <v>252</v>
+      </c>
+      <c r="V13" s="119"/>
+      <c r="W13" s="119"/>
+      <c r="X13" s="119"/>
+      <c r="Y13" s="119"/>
+      <c r="Z13" s="119"/>
       <c r="AA13" s="1"/>
       <c r="AB13" s="1"/>
       <c r="AC13" s="22"/>
       <c r="AD13" s="1"/>
-      <c r="AE13" s="1"/>
     </row>
     <row r="14" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C14" s="46">
@@ -7609,7 +7608,7 @@
       <c r="H14" s="87"/>
       <c r="I14" s="87"/>
       <c r="J14" s="124" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="K14" s="124"/>
       <c r="L14" s="124"/>
@@ -7623,16 +7622,16 @@
       <c r="R14" s="122" t="s">
         <v>228</v>
       </c>
-      <c r="S14" s="116"/>
-      <c r="T14" s="116"/>
-      <c r="U14" s="116" t="s">
-        <v>256</v>
-      </c>
-      <c r="V14" s="116"/>
-      <c r="W14" s="116"/>
-      <c r="X14" s="116"/>
-      <c r="Y14" s="116"/>
-      <c r="Z14" s="116"/>
+      <c r="S14" s="119"/>
+      <c r="T14" s="119"/>
+      <c r="U14" s="119" t="s">
+        <v>255</v>
+      </c>
+      <c r="V14" s="119"/>
+      <c r="W14" s="119"/>
+      <c r="X14" s="119"/>
+      <c r="Y14" s="119"/>
+      <c r="Z14" s="119"/>
       <c r="AA14" s="1"/>
       <c r="AB14" s="1"/>
       <c r="AC14" s="22"/>
@@ -7650,7 +7649,7 @@
       <c r="H15" s="87"/>
       <c r="I15" s="87"/>
       <c r="J15" s="124" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K15" s="124"/>
       <c r="L15" s="124"/>
@@ -7664,16 +7663,16 @@
       <c r="R15" s="122" t="s">
         <v>184</v>
       </c>
-      <c r="S15" s="116"/>
-      <c r="T15" s="116"/>
-      <c r="U15" s="116" t="s">
-        <v>257</v>
-      </c>
-      <c r="V15" s="116"/>
-      <c r="W15" s="116"/>
-      <c r="X15" s="116"/>
-      <c r="Y15" s="116"/>
-      <c r="Z15" s="116"/>
+      <c r="S15" s="119"/>
+      <c r="T15" s="119"/>
+      <c r="U15" s="119" t="s">
+        <v>256</v>
+      </c>
+      <c r="V15" s="119"/>
+      <c r="W15" s="119"/>
+      <c r="X15" s="119"/>
+      <c r="Y15" s="119"/>
+      <c r="Z15" s="119"/>
       <c r="AA15" s="1"/>
       <c r="AB15" s="1"/>
       <c r="AC15" s="22"/>
@@ -7716,7 +7715,7 @@
         <v>12</v>
       </c>
       <c r="D17" s="87" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E17" s="87"/>
       <c r="F17" s="87"/>
@@ -7724,7 +7723,7 @@
       <c r="H17" s="87"/>
       <c r="I17" s="87"/>
       <c r="J17" s="127" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="K17" s="127"/>
       <c r="L17" s="127"/>
@@ -7734,7 +7733,7 @@
       </c>
       <c r="O17" s="73"/>
       <c r="P17" s="123" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="Q17" s="123"/>
       <c r="R17" s="126" t="s">
@@ -7743,7 +7742,7 @@
       <c r="S17" s="126"/>
       <c r="T17" s="126"/>
       <c r="U17" s="73" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="V17" s="73"/>
       <c r="W17" s="73"/>
@@ -7778,7 +7777,7 @@
       <c r="S18" s="126"/>
       <c r="T18" s="126"/>
       <c r="U18" s="73" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="V18" s="73"/>
       <c r="W18" s="73"/>
@@ -7802,7 +7801,7 @@
       <c r="H19" s="87"/>
       <c r="I19" s="87"/>
       <c r="J19" s="69" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K19" s="69"/>
       <c r="L19" s="69"/>
@@ -7818,14 +7817,14 @@
       </c>
       <c r="S19" s="122"/>
       <c r="T19" s="122"/>
-      <c r="U19" s="116" t="s">
-        <v>264</v>
-      </c>
-      <c r="V19" s="116"/>
-      <c r="W19" s="116"/>
-      <c r="X19" s="116"/>
-      <c r="Y19" s="116"/>
-      <c r="Z19" s="116"/>
+      <c r="U19" s="119" t="s">
+        <v>263</v>
+      </c>
+      <c r="V19" s="119"/>
+      <c r="W19" s="119"/>
+      <c r="X19" s="119"/>
+      <c r="Y19" s="119"/>
+      <c r="Z19" s="119"/>
       <c r="AA19" s="68"/>
       <c r="AB19" s="67"/>
       <c r="AC19" s="67"/>
@@ -7876,7 +7875,7 @@
       <c r="H21" s="87"/>
       <c r="I21" s="87"/>
       <c r="J21" s="124" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="K21" s="124"/>
       <c r="L21" s="124"/>
@@ -7886,7 +7885,7 @@
       </c>
       <c r="O21" s="73"/>
       <c r="P21" s="123" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="Q21" s="123"/>
       <c r="R21" s="73" t="s">
@@ -7895,7 +7894,7 @@
       <c r="S21" s="73"/>
       <c r="T21" s="73"/>
       <c r="U21" s="125" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="V21" s="125"/>
       <c r="W21" s="125"/>
@@ -7919,7 +7918,7 @@
       <c r="H22" s="87"/>
       <c r="I22" s="87"/>
       <c r="J22" s="124" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K22" s="124"/>
       <c r="L22" s="124"/>
@@ -7930,19 +7929,19 @@
       <c r="O22" s="73"/>
       <c r="P22" s="123"/>
       <c r="Q22" s="123"/>
-      <c r="R22" s="116" t="s">
+      <c r="R22" s="119" t="s">
         <v>184</v>
       </c>
-      <c r="S22" s="116"/>
-      <c r="T22" s="116"/>
-      <c r="U22" s="116" t="s">
-        <v>269</v>
-      </c>
-      <c r="V22" s="116"/>
-      <c r="W22" s="116"/>
-      <c r="X22" s="116"/>
-      <c r="Y22" s="116"/>
-      <c r="Z22" s="116"/>
+      <c r="S22" s="119"/>
+      <c r="T22" s="119"/>
+      <c r="U22" s="119" t="s">
+        <v>268</v>
+      </c>
+      <c r="V22" s="119"/>
+      <c r="W22" s="119"/>
+      <c r="X22" s="119"/>
+      <c r="Y22" s="119"/>
+      <c r="Z22" s="119"/>
       <c r="AA22" s="22"/>
       <c r="AB22" s="1"/>
       <c r="AC22" s="1"/>
@@ -8123,7 +8122,7 @@
       <c r="M28" s="7"/>
       <c r="N28" s="7"/>
       <c r="O28" s="7"/>
-      <c r="P28" s="7"/>
+      <c r="P28" s="8"/>
       <c r="Q28" s="7"/>
       <c r="R28" s="7"/>
       <c r="S28" s="7"/>

</xml_diff>